<commit_message>
Implemeted Inventory Extract Report logic
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chaithra\APAC_796_Daily_Raw_Data\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DC4EC3-AFC9-41F1-812F-3578930FAC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB7698C-8431-47C4-A9F7-A76FE6708898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,14 @@
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Credentials" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -147,12 +148,6 @@
     <t>Static part of logging message. Error loading transaction data</t>
   </si>
   <si>
-    <t>Orchestrator Queue Name.</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
     <t>Process Name of the Automation(If you process automation from business side, you can include that)</t>
   </si>
   <si>
@@ -165,20 +160,35 @@
     <t>Daily Raw Data</t>
   </si>
   <si>
-    <t>796_Extract_Report</t>
-  </si>
-  <si>
     <t>796_GetEmail_Count</t>
   </si>
   <si>
     <t>796_Download_Reports_Path</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>796_JDE_Url</t>
+  </si>
+  <si>
+    <t>796_Role</t>
+  </si>
+  <si>
+    <t>796_Queue_Name</t>
+  </si>
+  <si>
+    <t>796_JDE_Credentials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -210,6 +220,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF464E55"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -241,6 +257,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -611,7 +628,7 @@
         <v>796</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -619,10 +636,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -630,7 +647,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -691,17 +708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1687,7 +1694,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2809,10 +2815,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB11BF1D-73C8-432F-835C-94674457BC78}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.08984375" defaultRowHeight="14.5"/>
@@ -2820,31 +2826,116 @@
     <col min="1" max="1" width="66.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="18.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3341E0-FB6F-4FE4-9A98-E6C0E829CED9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>